<commit_message>
added support to auto makedir for non-existent dir
</commit_message>
<xml_diff>
--- a/output_screener_us_long_SP500.xlsx
+++ b/output_screener_us_long_SP500.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
   <si>
     <t>Stock</t>
   </si>
@@ -52,100 +52,109 @@
     <t>% from 52 week high</t>
   </si>
   <si>
+    <t>MCK</t>
+  </si>
+  <si>
+    <t>IRM</t>
+  </si>
+  <si>
+    <t>TMUS</t>
+  </si>
+  <si>
     <t>ENPH</t>
   </si>
   <si>
-    <t>IRM</t>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>DVN</t>
   </si>
   <si>
     <t>CF</t>
   </si>
   <si>
-    <t>MCK</t>
-  </si>
-  <si>
     <t>NLSN</t>
   </si>
   <si>
-    <t>ED</t>
-  </si>
-  <si>
-    <t>TMUS</t>
+    <t>GWW</t>
+  </si>
+  <si>
+    <t>AZO</t>
+  </si>
+  <si>
+    <t>VRTX</t>
+  </si>
+  <si>
+    <t>MTB</t>
+  </si>
+  <si>
+    <t>NOC</t>
+  </si>
+  <si>
+    <t>PGR</t>
+  </si>
+  <si>
+    <t>GIS</t>
+  </si>
+  <si>
+    <t>CNC</t>
+  </si>
+  <si>
+    <t>GPC</t>
+  </si>
+  <si>
+    <t>SRE</t>
+  </si>
+  <si>
+    <t>CHRW</t>
+  </si>
+  <si>
+    <t>JKHY</t>
   </si>
   <si>
     <t>OXY</t>
   </si>
   <si>
-    <t>NOC</t>
-  </si>
-  <si>
-    <t>MTB</t>
-  </si>
-  <si>
-    <t>AZO</t>
-  </si>
-  <si>
-    <t>VRTX</t>
-  </si>
-  <si>
-    <t>GWW</t>
-  </si>
-  <si>
-    <t>PGR</t>
-  </si>
-  <si>
-    <t>CNC</t>
-  </si>
-  <si>
-    <t>GPC</t>
-  </si>
-  <si>
-    <t>SRE</t>
-  </si>
-  <si>
-    <t>CHRW</t>
-  </si>
-  <si>
     <t>CI</t>
   </si>
   <si>
-    <t>JKHY</t>
-  </si>
-  <si>
-    <t>DVN</t>
-  </si>
-  <si>
     <t>AJG</t>
   </si>
   <si>
     <t>PWR</t>
   </si>
   <si>
+    <t>CTVA</t>
+  </si>
+  <si>
+    <t>ATO</t>
+  </si>
+  <si>
     <t>LW</t>
   </si>
   <si>
+    <t>HSY</t>
+  </si>
+  <si>
+    <t>CAH</t>
+  </si>
+  <si>
     <t>ELV</t>
   </si>
   <si>
-    <t>CTVA</t>
+    <t>ULTA</t>
   </si>
   <si>
     <t>HII</t>
   </si>
   <si>
+    <t>RSG</t>
+  </si>
+  <si>
     <t>MOH</t>
   </si>
   <si>
-    <t>HSY</t>
-  </si>
-  <si>
-    <t>CAH</t>
-  </si>
-  <si>
-    <t>ATO</t>
-  </si>
-  <si>
-    <t>ULTA</t>
+    <t>UNH</t>
   </si>
   <si>
     <t>HWM</t>
@@ -154,49 +163,49 @@
     <t>CNP</t>
   </si>
   <si>
+    <t>HUM</t>
+  </si>
+  <si>
     <t>SO</t>
   </si>
   <si>
+    <t>AEP</t>
+  </si>
+  <si>
     <t>CTXS</t>
   </si>
   <si>
-    <t>AEP</t>
-  </si>
-  <si>
     <t>XOM</t>
   </si>
   <si>
-    <t>VLO</t>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+  <si>
+    <t>Communication Services</t>
   </si>
   <si>
     <t>Information Technology</t>
   </si>
   <si>
-    <t>Real Estate</t>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Energy</t>
   </si>
   <si>
     <t>Materials</t>
   </si>
   <si>
-    <t>Health Care</t>
-  </si>
-  <si>
     <t>Industrials</t>
   </si>
   <si>
-    <t>Utilities</t>
-  </si>
-  <si>
-    <t>Communication Services</t>
-  </si>
-  <si>
-    <t>Energy</t>
+    <t>Consumer Discretionary</t>
   </si>
   <si>
     <t>Financials</t>
-  </si>
-  <si>
-    <t>Consumer Discretionary</t>
   </si>
   <si>
     <t>Consumer Staples</t>
@@ -557,7 +566,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -606,37 +615,37 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2">
-        <v>1.93</v>
+        <v>1.78</v>
       </c>
       <c r="E2">
-        <v>305.7</v>
+        <v>363.73</v>
       </c>
       <c r="F2">
-        <v>-3.69</v>
+        <v>-0.68</v>
       </c>
       <c r="G2">
-        <v>259.93</v>
+        <v>347.48</v>
       </c>
       <c r="H2">
-        <v>203.33</v>
+        <v>319.44</v>
       </c>
       <c r="I2">
-        <v>197.34</v>
+        <v>299.77</v>
       </c>
       <c r="J2">
-        <v>113.4</v>
+        <v>193.89</v>
       </c>
       <c r="K2">
-        <v>324.84</v>
+        <v>375.23</v>
       </c>
       <c r="L2">
-        <v>5.89</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -644,28 +653,28 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>100</v>
       </c>
       <c r="D3">
-        <v>1.24</v>
+        <v>1.26</v>
       </c>
       <c r="E3">
-        <v>55.23</v>
+        <v>56.54</v>
       </c>
       <c r="F3">
-        <v>4.6</v>
+        <v>2.37</v>
       </c>
       <c r="G3">
-        <v>50.67</v>
+        <v>50.83</v>
       </c>
       <c r="H3">
-        <v>50.5</v>
+        <v>50.58</v>
       </c>
       <c r="I3">
-        <v>49.45</v>
+        <v>49.51</v>
       </c>
       <c r="J3">
         <v>41.67</v>
@@ -674,7 +683,7 @@
         <v>58.61</v>
       </c>
       <c r="L3">
-        <v>5.77</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -682,37 +691,37 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C4">
         <v>100</v>
       </c>
       <c r="D4">
-        <v>2.31</v>
+        <v>1.12</v>
       </c>
       <c r="E4">
-        <v>103.68</v>
+        <v>145.15</v>
       </c>
       <c r="F4">
-        <v>1.19</v>
+        <v>-0.38</v>
       </c>
       <c r="G4">
-        <v>96.67</v>
+        <v>141.46</v>
       </c>
       <c r="H4">
-        <v>94.15000000000001</v>
+        <v>132.76</v>
       </c>
       <c r="I4">
-        <v>87.11</v>
+        <v>127.81</v>
       </c>
       <c r="J4">
-        <v>44.83</v>
+        <v>101.51</v>
       </c>
       <c r="K4">
-        <v>119.6</v>
+        <v>148.04</v>
       </c>
       <c r="L4">
-        <v>13.31</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -720,37 +729,37 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
       <c r="D5">
-        <v>1.82</v>
+        <v>1.93</v>
       </c>
       <c r="E5">
-        <v>366.21</v>
+        <v>308.93</v>
       </c>
       <c r="F5">
-        <v>-1.07</v>
+        <v>1.06</v>
       </c>
       <c r="G5">
-        <v>346.72</v>
+        <v>262.2</v>
       </c>
       <c r="H5">
-        <v>318.77</v>
+        <v>204.45</v>
       </c>
       <c r="I5">
-        <v>299.08</v>
+        <v>197.63</v>
       </c>
       <c r="J5">
-        <v>193.89</v>
+        <v>113.4</v>
       </c>
       <c r="K5">
-        <v>375.23</v>
+        <v>324.84</v>
       </c>
       <c r="L5">
-        <v>2.4</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -758,7 +767,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -767,28 +776,28 @@
         <v>1.42</v>
       </c>
       <c r="E6">
-        <v>27.86</v>
+        <v>101.92</v>
       </c>
       <c r="F6">
-        <v>-0.04</v>
+        <v>1.06</v>
       </c>
       <c r="G6">
-        <v>25.46</v>
+        <v>96.51000000000001</v>
       </c>
       <c r="H6">
-        <v>24.03</v>
+        <v>92.91</v>
       </c>
       <c r="I6">
-        <v>23.01</v>
+        <v>89.95</v>
       </c>
       <c r="J6">
-        <v>16.02</v>
+        <v>71.52</v>
       </c>
       <c r="K6">
-        <v>27.92</v>
+        <v>102.21</v>
       </c>
       <c r="L6">
-        <v>0.21</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -796,37 +805,37 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
       <c r="D7">
-        <v>1.4</v>
+        <v>2.65</v>
       </c>
       <c r="E7">
-        <v>100.85</v>
+        <v>71.19</v>
       </c>
       <c r="F7">
-        <v>0.19</v>
+        <v>3.91</v>
       </c>
       <c r="G7">
-        <v>96.34999999999999</v>
+        <v>60.47</v>
       </c>
       <c r="H7">
-        <v>92.79000000000001</v>
+        <v>59.92</v>
       </c>
       <c r="I7">
-        <v>89.83</v>
+        <v>55.77</v>
       </c>
       <c r="J7">
-        <v>71.52</v>
+        <v>27.4</v>
       </c>
       <c r="K7">
-        <v>101.57</v>
+        <v>79.40000000000001</v>
       </c>
       <c r="L7">
-        <v>0.71</v>
+        <v>10.34</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -834,37 +843,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C8">
         <v>100</v>
       </c>
       <c r="D8">
-        <v>1.11</v>
+        <v>2.18</v>
       </c>
       <c r="E8">
-        <v>145.7</v>
+        <v>99.48</v>
       </c>
       <c r="F8">
-        <v>0.23</v>
+        <v>-4.05</v>
       </c>
       <c r="G8">
-        <v>141.25</v>
+        <v>96.95</v>
       </c>
       <c r="H8">
-        <v>132.59</v>
+        <v>94.31999999999999</v>
       </c>
       <c r="I8">
-        <v>127.66</v>
+        <v>87.28</v>
       </c>
       <c r="J8">
-        <v>101.51</v>
+        <v>45.52</v>
       </c>
       <c r="K8">
-        <v>148.04</v>
+        <v>119.6</v>
       </c>
       <c r="L8">
-        <v>1.58</v>
+        <v>16.82</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -872,37 +881,37 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9">
-        <v>2.64</v>
+        <v>1.39</v>
       </c>
       <c r="E9">
-        <v>65.61</v>
+        <v>27.86</v>
       </c>
       <c r="F9">
-        <v>1.75</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>64.13</v>
+        <v>25.55</v>
       </c>
       <c r="H9">
-        <v>59.08</v>
+        <v>24.1</v>
       </c>
       <c r="I9">
-        <v>52.31</v>
+        <v>23.04</v>
       </c>
       <c r="J9">
-        <v>24.94</v>
+        <v>16.02</v>
       </c>
       <c r="K9">
-        <v>77.13</v>
+        <v>27.92</v>
       </c>
       <c r="L9">
-        <v>14.94</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -910,37 +919,37 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>99</v>
       </c>
       <c r="D10">
-        <v>1.41</v>
+        <v>1.39</v>
       </c>
       <c r="E10">
-        <v>491.41</v>
+        <v>568.1</v>
       </c>
       <c r="F10">
-        <v>0.34</v>
+        <v>-0.8100000000000001</v>
       </c>
       <c r="G10">
-        <v>473.51</v>
+        <v>528.97</v>
       </c>
       <c r="H10">
-        <v>452.93</v>
+        <v>498.79</v>
       </c>
       <c r="I10">
-        <v>433.71</v>
+        <v>498.14</v>
       </c>
       <c r="J10">
-        <v>344.89</v>
+        <v>391.16</v>
       </c>
       <c r="K10">
-        <v>497.2</v>
+        <v>588.62</v>
       </c>
       <c r="L10">
-        <v>1.16</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -948,37 +957,37 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C11">
         <v>98</v>
       </c>
       <c r="D11">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="E11">
-        <v>187.61</v>
+        <v>2220.38</v>
       </c>
       <c r="F11">
-        <v>-0.15</v>
+        <v>0.97</v>
       </c>
       <c r="G11">
-        <v>173.98</v>
+        <v>2193.34</v>
       </c>
       <c r="H11">
-        <v>171.42</v>
+        <v>2069.45</v>
       </c>
       <c r="I11">
-        <v>167.99</v>
+        <v>2047.64</v>
       </c>
       <c r="J11">
-        <v>131.42</v>
+        <v>1540.98</v>
       </c>
       <c r="K11">
-        <v>193.42</v>
+        <v>2362.24</v>
       </c>
       <c r="L11">
-        <v>3</v>
+        <v>6.01</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -986,37 +995,37 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C12">
         <v>98</v>
       </c>
       <c r="D12">
-        <v>1.42</v>
+        <v>1.54</v>
       </c>
       <c r="E12">
-        <v>2199.08</v>
+        <v>293.48</v>
       </c>
       <c r="F12">
-        <v>0.27</v>
+        <v>0.47</v>
       </c>
       <c r="G12">
-        <v>2191.92</v>
+        <v>288.25</v>
       </c>
       <c r="H12">
-        <v>2068.11</v>
+        <v>267.83</v>
       </c>
       <c r="I12">
-        <v>2045.93</v>
+        <v>255.8</v>
       </c>
       <c r="J12">
-        <v>1540.98</v>
+        <v>176.36</v>
       </c>
       <c r="K12">
-        <v>2362.24</v>
+        <v>305.95</v>
       </c>
       <c r="L12">
-        <v>6.91</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1024,37 +1033,37 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C13">
         <v>98</v>
       </c>
       <c r="D13">
-        <v>1.55</v>
+        <v>1.43</v>
       </c>
       <c r="E13">
-        <v>292.11</v>
+        <v>190.55</v>
       </c>
       <c r="F13">
-        <v>1.08</v>
+        <v>1.57</v>
       </c>
       <c r="G13">
-        <v>288.02</v>
+        <v>174.63</v>
       </c>
       <c r="H13">
-        <v>267.48</v>
+        <v>171.52</v>
       </c>
       <c r="I13">
-        <v>255.27</v>
+        <v>168.15</v>
       </c>
       <c r="J13">
-        <v>176.36</v>
+        <v>131.42</v>
       </c>
       <c r="K13">
-        <v>305.95</v>
+        <v>193.42</v>
       </c>
       <c r="L13">
-        <v>4.52</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1062,37 +1071,37 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C14">
         <v>97</v>
       </c>
       <c r="D14">
-        <v>1.4</v>
+        <v>1.38</v>
       </c>
       <c r="E14">
-        <v>572.74</v>
+        <v>482.3</v>
       </c>
       <c r="F14">
-        <v>0.34</v>
+        <v>-1.85</v>
       </c>
       <c r="G14">
-        <v>526.67</v>
+        <v>473.62</v>
       </c>
       <c r="H14">
-        <v>498.22</v>
+        <v>453.71</v>
       </c>
       <c r="I14">
-        <v>497.77</v>
+        <v>434.33</v>
       </c>
       <c r="J14">
-        <v>391.16</v>
+        <v>344.89</v>
       </c>
       <c r="K14">
-        <v>588.62</v>
+        <v>497.2</v>
       </c>
       <c r="L14">
-        <v>2.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1100,37 +1109,37 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C15">
         <v>97</v>
       </c>
       <c r="D15">
-        <v>1.41</v>
+        <v>1.4</v>
       </c>
       <c r="E15">
-        <v>128.68</v>
+        <v>129.1</v>
       </c>
       <c r="F15">
-        <v>-0.42</v>
+        <v>0.33</v>
       </c>
       <c r="G15">
-        <v>119.55</v>
+        <v>119.8</v>
       </c>
       <c r="H15">
-        <v>114.01</v>
+        <v>114.15</v>
       </c>
       <c r="I15">
-        <v>111.02</v>
+        <v>111.2</v>
       </c>
       <c r="J15">
         <v>89.34999999999999</v>
       </c>
       <c r="K15">
-        <v>129.24</v>
+        <v>129.76</v>
       </c>
       <c r="L15">
-        <v>0.43</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1138,37 +1147,37 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C16">
         <v>97</v>
       </c>
       <c r="D16">
-        <v>1.54</v>
+        <v>1.34</v>
       </c>
       <c r="E16">
-        <v>91.98999999999999</v>
+        <v>76.15000000000001</v>
       </c>
       <c r="F16">
-        <v>0.8</v>
+        <v>0.32</v>
       </c>
       <c r="G16">
-        <v>91.43000000000001</v>
+        <v>75.94</v>
       </c>
       <c r="H16">
-        <v>86.11</v>
+        <v>70.56</v>
       </c>
       <c r="I16">
-        <v>84.2</v>
+        <v>69.31999999999999</v>
       </c>
       <c r="J16">
-        <v>59.67</v>
+        <v>57.47</v>
       </c>
       <c r="K16">
-        <v>98.53</v>
+        <v>78.54000000000001</v>
       </c>
       <c r="L16">
-        <v>6.64</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1176,37 +1185,37 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C17">
         <v>97</v>
       </c>
       <c r="D17">
-        <v>1.41</v>
+        <v>1.48</v>
       </c>
       <c r="E17">
-        <v>162.8</v>
+        <v>92.90000000000001</v>
       </c>
       <c r="F17">
-        <v>0.53</v>
+        <v>0.99</v>
       </c>
       <c r="G17">
-        <v>149</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="H17">
-        <v>135.43</v>
+        <v>86.19</v>
       </c>
       <c r="I17">
-        <v>134.57</v>
+        <v>84.29000000000001</v>
       </c>
       <c r="J17">
-        <v>115.63</v>
+        <v>59.84</v>
       </c>
       <c r="K17">
-        <v>163.5</v>
+        <v>98.53</v>
       </c>
       <c r="L17">
-        <v>0.43</v>
+        <v>5.71</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1214,37 +1223,37 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C18">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D18">
-        <v>1.35</v>
+        <v>1.4</v>
       </c>
       <c r="E18">
-        <v>173.76</v>
+        <v>163.15</v>
       </c>
       <c r="F18">
-        <v>0.47</v>
+        <v>0.21</v>
       </c>
       <c r="G18">
-        <v>160.82</v>
+        <v>149.62</v>
       </c>
       <c r="H18">
-        <v>156.51</v>
+        <v>135.67</v>
       </c>
       <c r="I18">
-        <v>149.51</v>
+        <v>134.72</v>
       </c>
       <c r="J18">
-        <v>119.56</v>
+        <v>115.63</v>
       </c>
       <c r="K18">
-        <v>174.88</v>
+        <v>164.99</v>
       </c>
       <c r="L18">
-        <v>0.64</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1252,37 +1261,37 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C19">
         <v>96</v>
       </c>
       <c r="D19">
-        <v>1.33</v>
+        <v>1.35</v>
       </c>
       <c r="E19">
-        <v>114.29</v>
+        <v>175.65</v>
       </c>
       <c r="F19">
-        <v>0.9399999999999999</v>
+        <v>1.09</v>
       </c>
       <c r="G19">
-        <v>108.24</v>
+        <v>161.35</v>
       </c>
       <c r="H19">
-        <v>103.7</v>
+        <v>156.79</v>
       </c>
       <c r="I19">
-        <v>103.09</v>
+        <v>149.78</v>
       </c>
       <c r="J19">
-        <v>85.8</v>
+        <v>119.56</v>
       </c>
       <c r="K19">
-        <v>121.23</v>
+        <v>176.47</v>
       </c>
       <c r="L19">
-        <v>5.72</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1290,37 +1299,37 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C20">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D20">
-        <v>1.46</v>
+        <v>1.31</v>
       </c>
       <c r="E20">
-        <v>292.84</v>
+        <v>113.55</v>
       </c>
       <c r="F20">
-        <v>0.73</v>
+        <v>-0.65</v>
       </c>
       <c r="G20">
-        <v>279.2</v>
+        <v>108.5</v>
       </c>
       <c r="H20">
-        <v>257.29</v>
+        <v>103.87</v>
       </c>
       <c r="I20">
-        <v>248.04</v>
+        <v>103.18</v>
       </c>
       <c r="J20">
-        <v>191.74</v>
+        <v>85.8</v>
       </c>
       <c r="K20">
-        <v>294.53</v>
+        <v>121.23</v>
       </c>
       <c r="L20">
-        <v>0.57</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1328,7 +1337,7 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C21">
         <v>95</v>
@@ -1337,19 +1346,19 @@
         <v>1.2</v>
       </c>
       <c r="E21">
-        <v>200.22</v>
+        <v>200.17</v>
       </c>
       <c r="F21">
-        <v>1.43</v>
+        <v>-0.02</v>
       </c>
       <c r="G21">
-        <v>197.58</v>
+        <v>197.99</v>
       </c>
       <c r="H21">
-        <v>188.12</v>
+        <v>188.34</v>
       </c>
       <c r="I21">
-        <v>181.52</v>
+        <v>181.76</v>
       </c>
       <c r="J21">
         <v>147.5</v>
@@ -1358,7 +1367,7 @@
         <v>212.62</v>
       </c>
       <c r="L21">
-        <v>5.83</v>
+        <v>5.86</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1366,37 +1375,37 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C22">
         <v>95</v>
       </c>
       <c r="D22">
-        <v>2.63</v>
+        <v>2.52</v>
       </c>
       <c r="E22">
-        <v>68.51000000000001</v>
+        <v>66.8</v>
       </c>
       <c r="F22">
-        <v>1.71</v>
+        <v>1.81</v>
       </c>
       <c r="G22">
-        <v>60.13</v>
+        <v>64.29000000000001</v>
       </c>
       <c r="H22">
-        <v>59.77</v>
+        <v>59.25</v>
       </c>
       <c r="I22">
-        <v>55.61</v>
+        <v>52.48</v>
       </c>
       <c r="J22">
-        <v>27.4</v>
+        <v>24.96</v>
       </c>
       <c r="K22">
-        <v>79.40000000000001</v>
+        <v>77.13</v>
       </c>
       <c r="L22">
-        <v>13.72</v>
+        <v>13.39</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1404,37 +1413,37 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C23">
         <v>95</v>
       </c>
       <c r="D23">
-        <v>1.32</v>
+        <v>1.43</v>
       </c>
       <c r="E23">
-        <v>188.42</v>
+        <v>294.15</v>
       </c>
       <c r="F23">
-        <v>0.71</v>
+        <v>0.45</v>
       </c>
       <c r="G23">
-        <v>176.97</v>
+        <v>279.84</v>
       </c>
       <c r="H23">
-        <v>167.38</v>
+        <v>257.79</v>
       </c>
       <c r="I23">
-        <v>165.93</v>
+        <v>248.47</v>
       </c>
       <c r="J23">
-        <v>142.53</v>
+        <v>191.74</v>
       </c>
       <c r="K23">
-        <v>192</v>
+        <v>296.29</v>
       </c>
       <c r="L23">
-        <v>1.86</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1442,37 +1451,37 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C24">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D24">
-        <v>1.27</v>
+        <v>1.32</v>
       </c>
       <c r="E24">
-        <v>146.76</v>
+        <v>187.63</v>
       </c>
       <c r="F24">
-        <v>0.1</v>
+        <v>-0.42</v>
       </c>
       <c r="G24">
-        <v>137.07</v>
+        <v>177.47</v>
       </c>
       <c r="H24">
-        <v>125.43</v>
+        <v>167.6</v>
       </c>
       <c r="I24">
-        <v>121.41</v>
+        <v>166.06</v>
       </c>
       <c r="J24">
-        <v>93.91</v>
+        <v>142.53</v>
       </c>
       <c r="K24">
-        <v>149.33</v>
+        <v>192</v>
       </c>
       <c r="L24">
-        <v>1.72</v>
+        <v>2.28</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1486,31 +1495,31 @@
         <v>94</v>
       </c>
       <c r="D25">
-        <v>1.33</v>
+        <v>1.27</v>
       </c>
       <c r="E25">
-        <v>79.5</v>
+        <v>145.66</v>
       </c>
       <c r="F25">
-        <v>0.06</v>
+        <v>-0.75</v>
       </c>
       <c r="G25">
-        <v>78.12</v>
+        <v>137.48</v>
       </c>
       <c r="H25">
-        <v>68.22</v>
+        <v>125.74</v>
       </c>
       <c r="I25">
-        <v>66.34999999999999</v>
+        <v>121.54</v>
       </c>
       <c r="J25">
-        <v>49.71</v>
+        <v>93.91</v>
       </c>
       <c r="K25">
-        <v>83.29000000000001</v>
+        <v>149.33</v>
       </c>
       <c r="L25">
-        <v>4.55</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1518,37 +1527,37 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C26">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26">
-        <v>1.4</v>
+        <v>1.46</v>
       </c>
       <c r="E26">
-        <v>493.6</v>
+        <v>62.11</v>
       </c>
       <c r="F26">
-        <v>0.87</v>
+        <v>-0.66</v>
       </c>
       <c r="G26">
-        <v>480.77</v>
+        <v>57.78</v>
       </c>
       <c r="H26">
-        <v>480.31</v>
+        <v>56.59</v>
       </c>
       <c r="I26">
-        <v>469.05</v>
+        <v>54.13</v>
       </c>
       <c r="J26">
-        <v>355.43</v>
+        <v>40.72</v>
       </c>
       <c r="K26">
-        <v>533.6799999999999</v>
+        <v>64.03</v>
       </c>
       <c r="L26">
-        <v>7.51</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1556,37 +1565,37 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C27">
         <v>93</v>
       </c>
       <c r="D27">
-        <v>1.46</v>
+        <v>1.33</v>
       </c>
       <c r="E27">
-        <v>62.52</v>
+        <v>119.44</v>
       </c>
       <c r="F27">
-        <v>0.77</v>
+        <v>1.14</v>
       </c>
       <c r="G27">
-        <v>57.61</v>
+        <v>114.99</v>
       </c>
       <c r="H27">
-        <v>56.51</v>
+        <v>113.17</v>
       </c>
       <c r="I27">
-        <v>54.06</v>
+        <v>109.74</v>
       </c>
       <c r="J27">
-        <v>40.72</v>
+        <v>85.8</v>
       </c>
       <c r="K27">
-        <v>64.03</v>
+        <v>122.96</v>
       </c>
       <c r="L27">
-        <v>2.36</v>
+        <v>2.86</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1594,37 +1603,37 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C28">
         <v>92</v>
       </c>
       <c r="D28">
-        <v>1.22</v>
+        <v>1.32</v>
       </c>
       <c r="E28">
-        <v>235.3</v>
+        <v>80.06</v>
       </c>
       <c r="F28">
-        <v>1.34</v>
+        <v>0.7</v>
       </c>
       <c r="G28">
-        <v>221.65</v>
+        <v>78.3</v>
       </c>
       <c r="H28">
-        <v>209.65</v>
+        <v>68.34</v>
       </c>
       <c r="I28">
-        <v>203.33</v>
+        <v>66.45999999999999</v>
       </c>
       <c r="J28">
-        <v>175.5</v>
+        <v>49.71</v>
       </c>
       <c r="K28">
-        <v>243.46</v>
+        <v>83.29000000000001</v>
       </c>
       <c r="L28">
-        <v>3.35</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1632,37 +1641,37 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C29">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D29">
-        <v>1.38</v>
+        <v>1.32</v>
       </c>
       <c r="E29">
-        <v>348.23</v>
+        <v>227.18</v>
       </c>
       <c r="F29">
-        <v>-1.47</v>
+        <v>0.41</v>
       </c>
       <c r="G29">
-        <v>317.13</v>
+        <v>223.84</v>
       </c>
       <c r="H29">
-        <v>311.8</v>
+        <v>215.96</v>
       </c>
       <c r="I29">
-        <v>307.95</v>
+        <v>209.1</v>
       </c>
       <c r="J29">
-        <v>249.57</v>
+        <v>167.8</v>
       </c>
       <c r="K29">
-        <v>361.25</v>
+        <v>234.56</v>
       </c>
       <c r="L29">
-        <v>3.6</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1670,37 +1679,37 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C30">
         <v>91</v>
       </c>
       <c r="D30">
-        <v>1.32</v>
+        <v>1.35</v>
       </c>
       <c r="E30">
-        <v>226.25</v>
+        <v>69.03</v>
       </c>
       <c r="F30">
-        <v>0.34</v>
+        <v>-1.23</v>
       </c>
       <c r="G30">
-        <v>223.58</v>
+        <v>62.35</v>
       </c>
       <c r="H30">
-        <v>215.78</v>
+        <v>57.64</v>
       </c>
       <c r="I30">
-        <v>208.86</v>
+        <v>55.56</v>
       </c>
       <c r="J30">
-        <v>167.8</v>
+        <v>45.85</v>
       </c>
       <c r="K30">
-        <v>234.56</v>
+        <v>72.28</v>
       </c>
       <c r="L30">
-        <v>3.54</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1711,34 +1720,34 @@
         <v>54</v>
       </c>
       <c r="C31">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D31">
-        <v>1.37</v>
+        <v>1.35</v>
       </c>
       <c r="E31">
-        <v>69.89</v>
+        <v>493.66</v>
       </c>
       <c r="F31">
-        <v>-1.05</v>
+        <v>0.01</v>
       </c>
       <c r="G31">
-        <v>62.01</v>
+        <v>481.02</v>
       </c>
       <c r="H31">
-        <v>57.52</v>
+        <v>480.65</v>
       </c>
       <c r="I31">
-        <v>55.46</v>
+        <v>469.42</v>
       </c>
       <c r="J31">
-        <v>45.85</v>
+        <v>358.39</v>
       </c>
       <c r="K31">
-        <v>72.28</v>
+        <v>533.6799999999999</v>
       </c>
       <c r="L31">
-        <v>3.31</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1746,37 +1755,37 @@
         <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C32">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D32">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="E32">
-        <v>118.09</v>
+        <v>446.14</v>
       </c>
       <c r="F32">
-        <v>0.12</v>
+        <v>0.73</v>
       </c>
       <c r="G32">
-        <v>114.83</v>
+        <v>400.77</v>
       </c>
       <c r="H32">
-        <v>113.06</v>
+        <v>393.38</v>
       </c>
       <c r="I32">
-        <v>109.61</v>
+        <v>391.23</v>
       </c>
       <c r="J32">
-        <v>85.8</v>
+        <v>330.8</v>
       </c>
       <c r="K32">
-        <v>122.96</v>
+        <v>451.3</v>
       </c>
       <c r="L32">
-        <v>3.96</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1784,37 +1793,37 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C33">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D33">
-        <v>1.18</v>
+        <v>1.2</v>
       </c>
       <c r="E33">
-        <v>442.9</v>
+        <v>235</v>
       </c>
       <c r="F33">
-        <v>-0.55</v>
+        <v>-0.13</v>
       </c>
       <c r="G33">
-        <v>399.55</v>
+        <v>222.01</v>
       </c>
       <c r="H33">
-        <v>392.85</v>
+        <v>210.02</v>
       </c>
       <c r="I33">
-        <v>391.05</v>
+        <v>203.58</v>
       </c>
       <c r="J33">
-        <v>330.8</v>
+        <v>175.5</v>
       </c>
       <c r="K33">
-        <v>448.29</v>
+        <v>243.46</v>
       </c>
       <c r="L33">
-        <v>1.2</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1822,37 +1831,37 @@
         <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C34">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D34">
-        <v>1.17</v>
+        <v>1.2</v>
       </c>
       <c r="E34">
-        <v>36.41</v>
+        <v>148.1</v>
       </c>
       <c r="F34">
-        <v>1.56</v>
+        <v>0.26</v>
       </c>
       <c r="G34">
-        <v>35.58</v>
+        <v>139.04</v>
       </c>
       <c r="H34">
-        <v>34.84</v>
+        <v>132.05</v>
       </c>
       <c r="I34">
-        <v>33.98</v>
+        <v>131.97</v>
       </c>
       <c r="J34">
-        <v>27.41</v>
+        <v>113.57</v>
       </c>
       <c r="K34">
-        <v>38.99</v>
+        <v>149.17</v>
       </c>
       <c r="L34">
-        <v>6.62</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1860,37 +1869,37 @@
         <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C35">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D35">
-        <v>1.28</v>
+        <v>1.33</v>
       </c>
       <c r="E35">
-        <v>32.85</v>
+        <v>349.36</v>
       </c>
       <c r="F35">
-        <v>0.46</v>
+        <v>0.32</v>
       </c>
       <c r="G35">
-        <v>31.02</v>
+        <v>318.53</v>
       </c>
       <c r="H35">
-        <v>30.04</v>
+        <v>312.14</v>
       </c>
       <c r="I35">
-        <v>29.27</v>
+        <v>308.16</v>
       </c>
       <c r="J35">
-        <v>24.33</v>
+        <v>249.78</v>
       </c>
       <c r="K35">
-        <v>33</v>
+        <v>361.25</v>
       </c>
       <c r="L35">
-        <v>0.45</v>
+        <v>3.29</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1898,37 +1907,37 @@
         <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C36">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D36">
-        <v>1.25</v>
+        <v>1.3</v>
       </c>
       <c r="E36">
-        <v>79.52</v>
+        <v>531.25</v>
       </c>
       <c r="F36">
-        <v>0.14</v>
+        <v>1.32</v>
       </c>
       <c r="G36">
-        <v>75.41</v>
+        <v>527.4400000000001</v>
       </c>
       <c r="H36">
-        <v>71.8</v>
+        <v>505.09</v>
       </c>
       <c r="I36">
-        <v>70.03</v>
+        <v>496.03</v>
       </c>
       <c r="J36">
-        <v>60.99</v>
+        <v>383.12</v>
       </c>
       <c r="K36">
-        <v>80.56999999999999</v>
+        <v>553.29</v>
       </c>
       <c r="L36">
-        <v>1.3</v>
+        <v>3.98</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1936,37 +1945,37 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C37">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="D37">
-        <v>0.97</v>
+        <v>1.15</v>
       </c>
       <c r="E37">
-        <v>103.68</v>
+        <v>37.02</v>
       </c>
       <c r="F37">
-        <v>-0.02</v>
+        <v>1.68</v>
       </c>
       <c r="G37">
-        <v>101.92</v>
+        <v>35.69</v>
       </c>
       <c r="H37">
-        <v>100.88</v>
+        <v>34.87</v>
       </c>
       <c r="I37">
-        <v>98.79000000000001</v>
+        <v>34.01</v>
       </c>
       <c r="J37">
-        <v>78.06999999999999</v>
+        <v>27.41</v>
       </c>
       <c r="K37">
-        <v>115</v>
+        <v>38.99</v>
       </c>
       <c r="L37">
-        <v>9.84</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1974,37 +1983,37 @@
         <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C38">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="D38">
-        <v>1.22</v>
+        <v>1.3</v>
       </c>
       <c r="E38">
-        <v>104.71</v>
+        <v>33.1</v>
       </c>
       <c r="F38">
-        <v>0.7</v>
+        <v>0.76</v>
       </c>
       <c r="G38">
-        <v>98.77</v>
+        <v>31.09</v>
       </c>
       <c r="H38">
-        <v>96.41</v>
+        <v>30.08</v>
       </c>
       <c r="I38">
-        <v>93.59999999999999</v>
+        <v>29.31</v>
       </c>
       <c r="J38">
-        <v>80.22</v>
+        <v>24.33</v>
       </c>
       <c r="K38">
-        <v>105.49</v>
+        <v>33.23</v>
       </c>
       <c r="L38">
-        <v>0.74</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2012,37 +2021,37 @@
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C39">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D39">
-        <v>1.87</v>
+        <v>1.2</v>
       </c>
       <c r="E39">
-        <v>96.5</v>
+        <v>486.14</v>
       </c>
       <c r="F39">
-        <v>1.68</v>
+        <v>1.6</v>
       </c>
       <c r="G39">
-        <v>90.76000000000001</v>
+        <v>485.84</v>
       </c>
       <c r="H39">
-        <v>87.03</v>
+        <v>454.53</v>
       </c>
       <c r="I39">
-        <v>81.39</v>
+        <v>446.31</v>
       </c>
       <c r="J39">
-        <v>52.96</v>
+        <v>351.2</v>
       </c>
       <c r="K39">
-        <v>105.57</v>
+        <v>504.99</v>
       </c>
       <c r="L39">
-        <v>8.59</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2053,34 +2062,148 @@
         <v>58</v>
       </c>
       <c r="C40">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D40">
-        <v>1.86</v>
+        <v>1.26</v>
       </c>
       <c r="E40">
-        <v>113.32</v>
+        <v>80.15000000000001</v>
       </c>
       <c r="F40">
-        <v>1.24</v>
+        <v>0.79</v>
       </c>
       <c r="G40">
-        <v>110.69</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="H40">
-        <v>107.41</v>
+        <v>71.88</v>
       </c>
       <c r="I40">
-        <v>99.02</v>
+        <v>70.13</v>
       </c>
       <c r="J40">
-        <v>61.86</v>
+        <v>60.99</v>
       </c>
       <c r="K40">
-        <v>146.81</v>
+        <v>80.56999999999999</v>
       </c>
       <c r="L40">
-        <v>22.81</v>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41">
+        <v>71</v>
+      </c>
+      <c r="D41">
+        <v>1.23</v>
+      </c>
+      <c r="E41">
+        <v>105.18</v>
+      </c>
+      <c r="F41">
+        <v>0.45</v>
+      </c>
+      <c r="G41">
+        <v>98.97</v>
+      </c>
+      <c r="H41">
+        <v>96.53</v>
+      </c>
+      <c r="I41">
+        <v>93.70999999999999</v>
+      </c>
+      <c r="J41">
+        <v>80.22</v>
+      </c>
+      <c r="K41">
+        <v>105.6</v>
+      </c>
+      <c r="L41">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42">
+        <v>68</v>
+      </c>
+      <c r="D42">
+        <v>0.96</v>
+      </c>
+      <c r="E42">
+        <v>103.67</v>
+      </c>
+      <c r="F42">
+        <v>-0.01</v>
+      </c>
+      <c r="G42">
+        <v>102.05</v>
+      </c>
+      <c r="H42">
+        <v>100.89</v>
+      </c>
+      <c r="I42">
+        <v>98.89</v>
+      </c>
+      <c r="J42">
+        <v>78.06999999999999</v>
+      </c>
+      <c r="K42">
+        <v>115</v>
+      </c>
+      <c r="L42">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43">
+        <v>67</v>
+      </c>
+      <c r="D43">
+        <v>1.84</v>
+      </c>
+      <c r="E43">
+        <v>97.61</v>
+      </c>
+      <c r="F43">
+        <v>1.15</v>
+      </c>
+      <c r="G43">
+        <v>91.01000000000001</v>
+      </c>
+      <c r="H43">
+        <v>87.15000000000001</v>
+      </c>
+      <c r="I43">
+        <v>81.56999999999999</v>
+      </c>
+      <c r="J43">
+        <v>52.96</v>
+      </c>
+      <c r="K43">
+        <v>105.57</v>
+      </c>
+      <c r="L43">
+        <v>7.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>